<commit_message>
update language import with automations for glottocodes
</commit_message>
<xml_diff>
--- a/app/static-files/language_import_template.xlsx
+++ b/app/static-files/language_import_template.xlsx
@@ -20,38 +20,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">ISO Indicator</t>
   </si>
   <si>
+    <t xml:space="preserve">Glottocode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Language Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternate Name(s)</t>
+    <t xml:space="preserve">Alternate name(s)</t>
   </si>
   <si>
     <t xml:space="preserve">Family</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary Subgroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Subgroup</t>
+    <t xml:space="preserve">Family abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family glottocode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary subgroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary subgroup abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary subgroup glottocode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary subgroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary subgroup abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary subgroup glottocode</t>
   </si>
   <si>
     <t xml:space="preserve">Dialects</t>
   </si>
   <si>
+    <t xml:space="preserve">Dialect glottocodes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Region</t>
   </si>
   <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
   <si>
+    <t xml:space="preserve">Comma separated list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Order of columns does not matter</t>
   </si>
   <si>
@@ -61,10 +100,7 @@
     <t xml:space="preserve">Column headers are case insensitive</t>
   </si>
   <si>
-    <t xml:space="preserve">Additional enumerated columns can be added (languages and dialects)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column headers in gray are supported but deprecated – they are supported mainly for backwards compatibility. They are preceded by the preferred headers.</t>
+    <t xml:space="preserve">Column headers in gray are for fields that will be automatically generated where possible. The automation will occur if a cell is empty or the column is omitted.</t>
   </si>
   <si>
     <t xml:space="preserve">This column can be deleted or ignored</t>
@@ -109,12 +145,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,120 +193,235 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1012" min="1" style="1" width="22.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1013" style="0" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1036" min="1024" style="2" width="22.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
+      <c r="A5" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
+      <c r="A6" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>